<commit_message>
readme, readings and distortion.io
</commit_message>
<xml_diff>
--- a/arduinoShit/potChange/50kresults.xlsx
+++ b/arduinoShit/potChange/50kresults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODING SHIT\tauri-app\arduinoShit\potChange\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2E66B29-D5B5-4506-8F69-5A8F4D63D626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA5FE8A-F15E-4CC6-AD1B-33BDAFBBA3D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="50kresults" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>Wiper Position</t>
   </si>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18">
     <font>
       <sz val="11"/>
@@ -3487,16 +3487,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>266698</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>397326</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>595312</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>174307</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>116340</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>174306</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3523,16 +3523,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>125730</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>185736</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>365216</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>33335</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>591503</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>45718</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>221389</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>78375</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3856,20 +3856,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AJ32" sqref="AJ32"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="22.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" customWidth="1"/>
+    <col min="6" max="6" width="23.44140625" customWidth="1"/>
+    <col min="7" max="7" width="22.21875" customWidth="1"/>
+    <col min="8" max="8" width="7.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3879,8 +3883,17 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3890,8 +3903,17 @@
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3901,8 +3923,17 @@
       <c r="C3">
         <v>39.200000000000003</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>505</v>
+      </c>
+      <c r="G3">
+        <v>39.200000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3912,8 +3943,17 @@
       <c r="C4">
         <v>88.2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>1010</v>
+      </c>
+      <c r="G4">
+        <v>88.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3923,8 +3963,17 @@
       <c r="C5">
         <v>142.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>1515</v>
+      </c>
+      <c r="G5">
+        <v>137.19999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3934,8 +3983,17 @@
       <c r="C6">
         <v>196</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>2020</v>
+      </c>
+      <c r="G6">
+        <v>186.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3945,8 +4003,17 @@
       <c r="C7">
         <v>240.1</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>2525</v>
+      </c>
+      <c r="G7">
+        <v>220.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3956,8 +4023,17 @@
       <c r="C8">
         <v>294</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>3030</v>
+      </c>
+      <c r="G8">
+        <v>274.39999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3967,8 +4043,17 @@
       <c r="C9">
         <v>338.1</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>3535</v>
+      </c>
+      <c r="G9">
+        <v>318.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3978,8 +4063,17 @@
       <c r="C10">
         <v>396.9</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <v>4040</v>
+      </c>
+      <c r="G10">
+        <v>362.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3989,8 +4083,17 @@
       <c r="C11">
         <v>445.9</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="E11">
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <v>4545</v>
+      </c>
+      <c r="G11">
+        <v>406.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4000,8 +4103,17 @@
       <c r="C12">
         <v>494.9</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>5050</v>
+      </c>
+      <c r="G12">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>11</v>
       </c>
@@ -4011,8 +4123,17 @@
       <c r="C13">
         <v>548.79999999999995</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="E13">
+        <v>11</v>
+      </c>
+      <c r="F13">
+        <v>5555</v>
+      </c>
+      <c r="G13">
+        <v>499.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>12</v>
       </c>
@@ -4022,8 +4143,17 @@
       <c r="C14">
         <v>592.9</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="E14">
+        <v>12</v>
+      </c>
+      <c r="F14">
+        <v>6060</v>
+      </c>
+      <c r="G14">
+        <v>534.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>13</v>
       </c>
@@ -4033,8 +4163,17 @@
       <c r="C15">
         <v>646.79999999999995</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="E15">
+        <v>13</v>
+      </c>
+      <c r="F15">
+        <v>6565</v>
+      </c>
+      <c r="G15">
+        <v>573.29999999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>14</v>
       </c>
@@ -4044,8 +4183,17 @@
       <c r="C16">
         <v>695.8</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="E16">
+        <v>14</v>
+      </c>
+      <c r="F16">
+        <v>7070</v>
+      </c>
+      <c r="G16">
+        <v>622.29999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>15</v>
       </c>
@@ -4055,8 +4203,17 @@
       <c r="C17">
         <v>749.7</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="E17">
+        <v>15</v>
+      </c>
+      <c r="F17">
+        <v>7575</v>
+      </c>
+      <c r="G17">
+        <v>656.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>16</v>
       </c>
@@ -4066,8 +4223,17 @@
       <c r="C18">
         <v>798.7</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="E18">
+        <v>16</v>
+      </c>
+      <c r="F18">
+        <v>8080</v>
+      </c>
+      <c r="G18">
+        <v>695.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>17</v>
       </c>
@@ -4077,8 +4243,17 @@
       <c r="C19">
         <v>847.7</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="E19">
+        <v>17</v>
+      </c>
+      <c r="F19">
+        <v>8585</v>
+      </c>
+      <c r="G19">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>18</v>
       </c>
@@ -4088,8 +4263,17 @@
       <c r="C20">
         <v>896.7</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="E20">
+        <v>18</v>
+      </c>
+      <c r="F20">
+        <v>9090</v>
+      </c>
+      <c r="G20">
+        <v>774.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>19</v>
       </c>
@@ -4099,8 +4283,17 @@
       <c r="C21">
         <v>950.6</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="E21">
+        <v>19</v>
+      </c>
+      <c r="F21">
+        <v>9595</v>
+      </c>
+      <c r="G21">
+        <v>813.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>20</v>
       </c>
@@ -4110,8 +4303,17 @@
       <c r="C22">
         <v>1004.5</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="E22">
+        <v>20</v>
+      </c>
+      <c r="F22">
+        <v>10101</v>
+      </c>
+      <c r="G22">
+        <v>852.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23">
         <v>21</v>
       </c>
@@ -4121,8 +4323,17 @@
       <c r="C23">
         <v>1043.7</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="E23">
+        <v>21</v>
+      </c>
+      <c r="F23">
+        <v>10606</v>
+      </c>
+      <c r="G23">
+        <v>896.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24">
         <v>22</v>
       </c>
@@ -4132,8 +4343,17 @@
       <c r="C24">
         <v>1097.5999999999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="E24">
+        <v>22</v>
+      </c>
+      <c r="F24">
+        <v>11111</v>
+      </c>
+      <c r="G24">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>23</v>
       </c>
@@ -4143,8 +4363,17 @@
       <c r="C25">
         <v>1151.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="E25">
+        <v>23</v>
+      </c>
+      <c r="F25">
+        <v>11616</v>
+      </c>
+      <c r="G25">
+        <v>970.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26">
         <v>24</v>
       </c>
@@ -4154,8 +4383,17 @@
       <c r="C26">
         <v>1200.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="E26">
+        <v>24</v>
+      </c>
+      <c r="F26">
+        <v>12121</v>
+      </c>
+      <c r="G26">
+        <v>1004.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27">
         <v>25</v>
       </c>
@@ -4165,8 +4403,17 @@
       <c r="C27">
         <v>1254.4000000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="E27">
+        <v>25</v>
+      </c>
+      <c r="F27">
+        <v>12626</v>
+      </c>
+      <c r="G27">
+        <v>1048.5999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28">
         <v>26</v>
       </c>
@@ -4176,8 +4423,17 @@
       <c r="C28">
         <v>1303.4000000000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="E28">
+        <v>26</v>
+      </c>
+      <c r="F28">
+        <v>13131</v>
+      </c>
+      <c r="G28">
+        <v>1082.9000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29">
         <v>27</v>
       </c>
@@ -4187,8 +4443,17 @@
       <c r="C29">
         <v>1352.4</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="E29">
+        <v>27</v>
+      </c>
+      <c r="F29">
+        <v>13636</v>
+      </c>
+      <c r="G29">
+        <v>1122.0999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30">
         <v>28</v>
       </c>
@@ -4198,8 +4463,17 @@
       <c r="C30">
         <v>1401.4</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="E30">
+        <v>28</v>
+      </c>
+      <c r="F30">
+        <v>14141</v>
+      </c>
+      <c r="G30">
+        <v>1156.4000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31">
         <v>29</v>
       </c>
@@ -4209,8 +4483,17 @@
       <c r="C31">
         <v>1460.2</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="E31">
+        <v>29</v>
+      </c>
+      <c r="F31">
+        <v>14646</v>
+      </c>
+      <c r="G31">
+        <v>1190.7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32">
         <v>30</v>
       </c>
@@ -4220,8 +4503,17 @@
       <c r="C32">
         <v>1504.3</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="E32">
+        <v>30</v>
+      </c>
+      <c r="F32">
+        <v>15151</v>
+      </c>
+      <c r="G32">
+        <v>1234.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33">
         <v>31</v>
       </c>
@@ -4231,8 +4523,17 @@
       <c r="C33">
         <v>1558.2</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="E33">
+        <v>31</v>
+      </c>
+      <c r="F33">
+        <v>15656</v>
+      </c>
+      <c r="G33">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34">
         <v>32</v>
       </c>
@@ -4242,8 +4543,17 @@
       <c r="C34">
         <v>1607.2</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="E34">
+        <v>32</v>
+      </c>
+      <c r="F34">
+        <v>16161</v>
+      </c>
+      <c r="G34">
+        <v>1308.3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35">
         <v>33</v>
       </c>
@@ -4253,8 +4563,17 @@
       <c r="C35">
         <v>1656.2</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="E35">
+        <v>33</v>
+      </c>
+      <c r="F35">
+        <v>16666</v>
+      </c>
+      <c r="G35">
+        <v>1342.6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36">
         <v>34</v>
       </c>
@@ -4264,8 +4583,17 @@
       <c r="C36">
         <v>1705.2</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="E36">
+        <v>34</v>
+      </c>
+      <c r="F36">
+        <v>17171</v>
+      </c>
+      <c r="G36">
+        <v>1381.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37">
         <v>35</v>
       </c>
@@ -4275,8 +4603,17 @@
       <c r="C37">
         <v>1759.1</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="E37">
+        <v>35</v>
+      </c>
+      <c r="F37">
+        <v>17676</v>
+      </c>
+      <c r="G37">
+        <v>1416.1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38">
         <v>36</v>
       </c>
@@ -4286,8 +4623,17 @@
       <c r="C38">
         <v>1808.1</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="E38">
+        <v>36</v>
+      </c>
+      <c r="F38">
+        <v>18181</v>
+      </c>
+      <c r="G38">
+        <v>1455.3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39">
         <v>37</v>
       </c>
@@ -4297,8 +4643,17 @@
       <c r="C39">
         <v>1852.2</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
+      <c r="E39">
+        <v>37</v>
+      </c>
+      <c r="F39">
+        <v>18686</v>
+      </c>
+      <c r="G39">
+        <v>1499.4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40">
         <v>38</v>
       </c>
@@ -4308,8 +4663,17 @@
       <c r="C40">
         <v>1911</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="E40">
+        <v>38</v>
+      </c>
+      <c r="F40">
+        <v>19191</v>
+      </c>
+      <c r="G40">
+        <v>1528.8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41">
         <v>39</v>
       </c>
@@ -4319,8 +4683,17 @@
       <c r="C41">
         <v>1960</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="E41">
+        <v>39</v>
+      </c>
+      <c r="F41">
+        <v>19696</v>
+      </c>
+      <c r="G41">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42">
         <v>40</v>
       </c>
@@ -4330,8 +4703,17 @@
       <c r="C42">
         <v>2009</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="E42">
+        <v>40</v>
+      </c>
+      <c r="F42">
+        <v>20202</v>
+      </c>
+      <c r="G42">
+        <v>1607.2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43">
         <v>41</v>
       </c>
@@ -4341,8 +4723,17 @@
       <c r="C43">
         <v>2062.9</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="E43">
+        <v>41</v>
+      </c>
+      <c r="F43">
+        <v>20707</v>
+      </c>
+      <c r="G43">
+        <v>1651.3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44">
         <v>42</v>
       </c>
@@ -4352,8 +4743,17 @@
       <c r="C44">
         <v>2107</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="E44">
+        <v>42</v>
+      </c>
+      <c r="F44">
+        <v>21212</v>
+      </c>
+      <c r="G44">
+        <v>1685.6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45">
         <v>43</v>
       </c>
@@ -4363,8 +4763,17 @@
       <c r="C45">
         <v>2160.9</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="E45">
+        <v>43</v>
+      </c>
+      <c r="F45">
+        <v>21717</v>
+      </c>
+      <c r="G45">
+        <v>1724.8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46">
         <v>44</v>
       </c>
@@ -4374,8 +4783,17 @@
       <c r="C46">
         <v>2209.9</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="E46">
+        <v>44</v>
+      </c>
+      <c r="F46">
+        <v>22222</v>
+      </c>
+      <c r="G46">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47">
         <v>45</v>
       </c>
@@ -4385,8 +4803,17 @@
       <c r="C47">
         <v>2263.8000000000002</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="E47">
+        <v>45</v>
+      </c>
+      <c r="F47">
+        <v>22727</v>
+      </c>
+      <c r="G47">
+        <v>1803.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48">
         <v>46</v>
       </c>
@@ -4396,8 +4823,17 @@
       <c r="C48">
         <v>2317.6999999999998</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
+      <c r="E48">
+        <v>46</v>
+      </c>
+      <c r="F48">
+        <v>23232</v>
+      </c>
+      <c r="G48">
+        <v>1837.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49">
         <v>47</v>
       </c>
@@ -4407,8 +4843,17 @@
       <c r="C49">
         <v>2361.8000000000002</v>
       </c>
-    </row>
-    <row r="50" spans="1:3">
+      <c r="E49">
+        <v>47</v>
+      </c>
+      <c r="F49">
+        <v>23737</v>
+      </c>
+      <c r="G49">
+        <v>1876.7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50">
         <v>48</v>
       </c>
@@ -4418,8 +4863,17 @@
       <c r="C50">
         <v>2415.6999999999998</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
+      <c r="E50">
+        <v>48</v>
+      </c>
+      <c r="F50">
+        <v>24242</v>
+      </c>
+      <c r="G50">
+        <v>1920.8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51">
         <v>49</v>
       </c>
@@ -4429,8 +4883,17 @@
       <c r="C51">
         <v>2459.8000000000002</v>
       </c>
-    </row>
-    <row r="52" spans="1:3">
+      <c r="E51">
+        <v>49</v>
+      </c>
+      <c r="F51">
+        <v>24747</v>
+      </c>
+      <c r="G51">
+        <v>1950.2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52">
         <v>50</v>
       </c>
@@ -4440,8 +4903,17 @@
       <c r="C52">
         <v>2513.6999999999998</v>
       </c>
-    </row>
-    <row r="53" spans="1:3">
+      <c r="E52">
+        <v>50</v>
+      </c>
+      <c r="F52">
+        <v>25252</v>
+      </c>
+      <c r="G52">
+        <v>1989.4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53">
         <v>51</v>
       </c>
@@ -4451,8 +4923,17 @@
       <c r="C53">
         <v>2562.6999999999998</v>
       </c>
-    </row>
-    <row r="54" spans="1:3">
+      <c r="E53">
+        <v>51</v>
+      </c>
+      <c r="F53">
+        <v>25757</v>
+      </c>
+      <c r="G53">
+        <v>2038.4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54">
         <v>52</v>
       </c>
@@ -4462,8 +4943,17 @@
       <c r="C54">
         <v>2616.6</v>
       </c>
-    </row>
-    <row r="55" spans="1:3">
+      <c r="E54">
+        <v>52</v>
+      </c>
+      <c r="F54">
+        <v>26262</v>
+      </c>
+      <c r="G54">
+        <v>2077.6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55">
         <v>53</v>
       </c>
@@ -4473,8 +4963,17 @@
       <c r="C55">
         <v>2665.6</v>
       </c>
-    </row>
-    <row r="56" spans="1:3">
+      <c r="E55">
+        <v>53</v>
+      </c>
+      <c r="F55">
+        <v>26767</v>
+      </c>
+      <c r="G55">
+        <v>2121.6999999999998</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56">
         <v>54</v>
       </c>
@@ -4484,8 +4983,17 @@
       <c r="C56">
         <v>2719.5</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
+      <c r="E56">
+        <v>54</v>
+      </c>
+      <c r="F56">
+        <v>27272</v>
+      </c>
+      <c r="G56">
+        <v>2170.6999999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57">
         <v>55</v>
       </c>
@@ -4495,8 +5003,17 @@
       <c r="C57">
         <v>2768.5</v>
       </c>
-    </row>
-    <row r="58" spans="1:3">
+      <c r="E57">
+        <v>55</v>
+      </c>
+      <c r="F57">
+        <v>27777</v>
+      </c>
+      <c r="G57">
+        <v>2205</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58">
         <v>56</v>
       </c>
@@ -4506,8 +5023,17 @@
       <c r="C58">
         <v>2822.4</v>
       </c>
-    </row>
-    <row r="59" spans="1:3">
+      <c r="E58">
+        <v>56</v>
+      </c>
+      <c r="F58">
+        <v>28282</v>
+      </c>
+      <c r="G58">
+        <v>2249.1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59">
         <v>57</v>
       </c>
@@ -4517,8 +5043,17 @@
       <c r="C59">
         <v>2871.4</v>
       </c>
-    </row>
-    <row r="60" spans="1:3">
+      <c r="E59">
+        <v>57</v>
+      </c>
+      <c r="F59">
+        <v>28787</v>
+      </c>
+      <c r="G59">
+        <v>2288.3000000000002</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60">
         <v>58</v>
       </c>
@@ -4528,8 +5063,17 @@
       <c r="C60">
         <v>2925.3</v>
       </c>
-    </row>
-    <row r="61" spans="1:3">
+      <c r="E60">
+        <v>58</v>
+      </c>
+      <c r="F60">
+        <v>29292</v>
+      </c>
+      <c r="G60">
+        <v>2332.4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61">
         <v>59</v>
       </c>
@@ -4539,8 +5083,17 @@
       <c r="C61">
         <v>2974.3</v>
       </c>
-    </row>
-    <row r="62" spans="1:3">
+      <c r="E61">
+        <v>59</v>
+      </c>
+      <c r="F61">
+        <v>29797</v>
+      </c>
+      <c r="G61">
+        <v>2376.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62">
         <v>60</v>
       </c>
@@ -4550,8 +5103,17 @@
       <c r="C62">
         <v>3023.3</v>
       </c>
-    </row>
-    <row r="63" spans="1:3">
+      <c r="E62">
+        <v>60</v>
+      </c>
+      <c r="F62">
+        <v>30303</v>
+      </c>
+      <c r="G62">
+        <v>2420.6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63">
         <v>61</v>
       </c>
@@ -4561,8 +5123,17 @@
       <c r="C63">
         <v>3072.3</v>
       </c>
-    </row>
-    <row r="64" spans="1:3">
+      <c r="E63">
+        <v>61</v>
+      </c>
+      <c r="F63">
+        <v>30808</v>
+      </c>
+      <c r="G63">
+        <v>2464.6999999999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64">
         <v>62</v>
       </c>
@@ -4572,8 +5143,17 @@
       <c r="C64">
         <v>3121.3</v>
       </c>
-    </row>
-    <row r="65" spans="1:3">
+      <c r="E64">
+        <v>62</v>
+      </c>
+      <c r="F64">
+        <v>31313</v>
+      </c>
+      <c r="G64">
+        <v>2513.6999999999998</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65">
         <v>63</v>
       </c>
@@ -4583,8 +5163,17 @@
       <c r="C65">
         <v>3175.2</v>
       </c>
-    </row>
-    <row r="66" spans="1:3">
+      <c r="E65">
+        <v>63</v>
+      </c>
+      <c r="F65">
+        <v>31818</v>
+      </c>
+      <c r="G65">
+        <v>2557.8000000000002</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66">
         <v>64</v>
       </c>
@@ -4594,8 +5183,17 @@
       <c r="C66">
         <v>3224.2</v>
       </c>
-    </row>
-    <row r="67" spans="1:3">
+      <c r="E66">
+        <v>64</v>
+      </c>
+      <c r="F66">
+        <v>32323</v>
+      </c>
+      <c r="G66">
+        <v>2606.8000000000002</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67">
         <v>65</v>
       </c>
@@ -4605,8 +5203,17 @@
       <c r="C67">
         <v>3273.2</v>
       </c>
-    </row>
-    <row r="68" spans="1:3">
+      <c r="E67">
+        <v>65</v>
+      </c>
+      <c r="F67">
+        <v>32828</v>
+      </c>
+      <c r="G67">
+        <v>2650.9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68">
         <v>66</v>
       </c>
@@ -4616,8 +5223,17 @@
       <c r="C68">
         <v>3322.2</v>
       </c>
-    </row>
-    <row r="69" spans="1:3">
+      <c r="E68">
+        <v>66</v>
+      </c>
+      <c r="F68">
+        <v>33333</v>
+      </c>
+      <c r="G68">
+        <v>2699.9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69">
         <v>67</v>
       </c>
@@ -4627,8 +5243,17 @@
       <c r="C69">
         <v>3376.1</v>
       </c>
-    </row>
-    <row r="70" spans="1:3">
+      <c r="E69">
+        <v>67</v>
+      </c>
+      <c r="F69">
+        <v>33838</v>
+      </c>
+      <c r="G69">
+        <v>2748.9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70">
         <v>68</v>
       </c>
@@ -4638,8 +5263,17 @@
       <c r="C70">
         <v>3425.1</v>
       </c>
-    </row>
-    <row r="71" spans="1:3">
+      <c r="E70">
+        <v>68</v>
+      </c>
+      <c r="F70">
+        <v>34343</v>
+      </c>
+      <c r="G70">
+        <v>2802.8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71">
         <v>69</v>
       </c>
@@ -4649,8 +5283,17 @@
       <c r="C71">
         <v>3479</v>
       </c>
-    </row>
-    <row r="72" spans="1:3">
+      <c r="E71">
+        <v>69</v>
+      </c>
+      <c r="F71">
+        <v>34848</v>
+      </c>
+      <c r="G71">
+        <v>2846.9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72">
         <v>70</v>
       </c>
@@ -4660,8 +5303,17 @@
       <c r="C72">
         <v>3528</v>
       </c>
-    </row>
-    <row r="73" spans="1:3">
+      <c r="E72">
+        <v>70</v>
+      </c>
+      <c r="F72">
+        <v>35353</v>
+      </c>
+      <c r="G72">
+        <v>2900.8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73">
         <v>71</v>
       </c>
@@ -4671,8 +5323,17 @@
       <c r="C73">
         <v>3581.9</v>
       </c>
-    </row>
-    <row r="74" spans="1:3">
+      <c r="E73">
+        <v>71</v>
+      </c>
+      <c r="F73">
+        <v>35858</v>
+      </c>
+      <c r="G73">
+        <v>2949.8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74">
         <v>72</v>
       </c>
@@ -4682,8 +5343,17 @@
       <c r="C74">
         <v>3630.9</v>
       </c>
-    </row>
-    <row r="75" spans="1:3">
+      <c r="E74">
+        <v>72</v>
+      </c>
+      <c r="F74">
+        <v>36363</v>
+      </c>
+      <c r="G74">
+        <v>3008.6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75">
         <v>73</v>
       </c>
@@ -4693,8 +5363,17 @@
       <c r="C75">
         <v>3679.9</v>
       </c>
-    </row>
-    <row r="76" spans="1:3">
+      <c r="E75">
+        <v>73</v>
+      </c>
+      <c r="F75">
+        <v>36868</v>
+      </c>
+      <c r="G75">
+        <v>3057.6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76">
         <v>74</v>
       </c>
@@ -4704,8 +5383,17 @@
       <c r="C76">
         <v>3728.9</v>
       </c>
-    </row>
-    <row r="77" spans="1:3">
+      <c r="E76">
+        <v>74</v>
+      </c>
+      <c r="F76">
+        <v>37373</v>
+      </c>
+      <c r="G76">
+        <v>3116.4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77">
         <v>75</v>
       </c>
@@ -4715,8 +5403,17 @@
       <c r="C77">
         <v>3777.9</v>
       </c>
-    </row>
-    <row r="78" spans="1:3">
+      <c r="E77">
+        <v>75</v>
+      </c>
+      <c r="F77">
+        <v>37878</v>
+      </c>
+      <c r="G77">
+        <v>3170.3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
       <c r="A78">
         <v>76</v>
       </c>
@@ -4726,8 +5423,17 @@
       <c r="C78">
         <v>3831.8</v>
       </c>
-    </row>
-    <row r="79" spans="1:3">
+      <c r="E78">
+        <v>76</v>
+      </c>
+      <c r="F78">
+        <v>38383</v>
+      </c>
+      <c r="G78">
+        <v>3224.2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79">
         <v>77</v>
       </c>
@@ -4737,8 +5443,17 @@
       <c r="C79">
         <v>3880.8</v>
       </c>
-    </row>
-    <row r="80" spans="1:3">
+      <c r="E79">
+        <v>77</v>
+      </c>
+      <c r="F79">
+        <v>38888</v>
+      </c>
+      <c r="G79">
+        <v>3287.9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80">
         <v>78</v>
       </c>
@@ -4748,8 +5463,17 @@
       <c r="C80">
         <v>3934.7</v>
       </c>
-    </row>
-    <row r="81" spans="1:3">
+      <c r="E80">
+        <v>78</v>
+      </c>
+      <c r="F80">
+        <v>39393</v>
+      </c>
+      <c r="G80">
+        <v>3346.7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81">
         <v>79</v>
       </c>
@@ -4759,8 +5483,17 @@
       <c r="C81">
         <v>3983.7</v>
       </c>
-    </row>
-    <row r="82" spans="1:3">
+      <c r="E81">
+        <v>79</v>
+      </c>
+      <c r="F81">
+        <v>39898</v>
+      </c>
+      <c r="G81">
+        <v>3410.4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82">
         <v>80</v>
       </c>
@@ -4770,8 +5503,17 @@
       <c r="C82">
         <v>4032.7</v>
       </c>
-    </row>
-    <row r="83" spans="1:3">
+      <c r="E82">
+        <v>80</v>
+      </c>
+      <c r="F82">
+        <v>40404</v>
+      </c>
+      <c r="G82">
+        <v>3469.2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83">
         <v>81</v>
       </c>
@@ -4781,8 +5523,17 @@
       <c r="C83">
         <v>4086.6</v>
       </c>
-    </row>
-    <row r="84" spans="1:3">
+      <c r="E83">
+        <v>81</v>
+      </c>
+      <c r="F83">
+        <v>40909</v>
+      </c>
+      <c r="G83">
+        <v>3532.9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
       <c r="A84">
         <v>82</v>
       </c>
@@ -4792,8 +5543,17 @@
       <c r="C84">
         <v>4135.6000000000004</v>
       </c>
-    </row>
-    <row r="85" spans="1:3">
+      <c r="E84">
+        <v>82</v>
+      </c>
+      <c r="F84">
+        <v>41414</v>
+      </c>
+      <c r="G84">
+        <v>3596.6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85">
         <v>83</v>
       </c>
@@ -4803,8 +5563,17 @@
       <c r="C85">
         <v>4179.7</v>
       </c>
-    </row>
-    <row r="86" spans="1:3">
+      <c r="E85">
+        <v>83</v>
+      </c>
+      <c r="F85">
+        <v>41919</v>
+      </c>
+      <c r="G85">
+        <v>3665.2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86">
         <v>84</v>
       </c>
@@ -4814,8 +5583,17 @@
       <c r="C86">
         <v>4233.6000000000004</v>
       </c>
-    </row>
-    <row r="87" spans="1:3">
+      <c r="E86">
+        <v>84</v>
+      </c>
+      <c r="F86">
+        <v>42424</v>
+      </c>
+      <c r="G86">
+        <v>3733.8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
       <c r="A87">
         <v>85</v>
       </c>
@@ -4825,8 +5603,17 @@
       <c r="C87">
         <v>4287.5</v>
       </c>
-    </row>
-    <row r="88" spans="1:3">
+      <c r="E87">
+        <v>85</v>
+      </c>
+      <c r="F87">
+        <v>42929</v>
+      </c>
+      <c r="G87">
+        <v>3802.4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88">
         <v>86</v>
       </c>
@@ -4836,8 +5623,17 @@
       <c r="C88">
         <v>4321.8</v>
       </c>
-    </row>
-    <row r="89" spans="1:3">
+      <c r="E88">
+        <v>86</v>
+      </c>
+      <c r="F88">
+        <v>43434</v>
+      </c>
+      <c r="G88">
+        <v>3871</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89">
         <v>87</v>
       </c>
@@ -4847,8 +5643,17 @@
       <c r="C89">
         <v>4385.5</v>
       </c>
-    </row>
-    <row r="90" spans="1:3">
+      <c r="E89">
+        <v>87</v>
+      </c>
+      <c r="F89">
+        <v>43939</v>
+      </c>
+      <c r="G89">
+        <v>3944.5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
       <c r="A90">
         <v>88</v>
       </c>
@@ -4858,8 +5663,17 @@
       <c r="C90">
         <v>4419.8</v>
       </c>
-    </row>
-    <row r="91" spans="1:3">
+      <c r="E90">
+        <v>88</v>
+      </c>
+      <c r="F90">
+        <v>44444</v>
+      </c>
+      <c r="G90">
+        <v>4018</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91">
         <v>89</v>
       </c>
@@ -4869,8 +5683,17 @@
       <c r="C91">
         <v>4483.5</v>
       </c>
-    </row>
-    <row r="92" spans="1:3">
+      <c r="E91">
+        <v>89</v>
+      </c>
+      <c r="F91">
+        <v>44949</v>
+      </c>
+      <c r="G91">
+        <v>4091.5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
       <c r="A92">
         <v>90</v>
       </c>
@@ -4880,8 +5703,17 @@
       <c r="C92">
         <v>4527.6000000000004</v>
       </c>
-    </row>
-    <row r="93" spans="1:3">
+      <c r="E92">
+        <v>90</v>
+      </c>
+      <c r="F92">
+        <v>45454</v>
+      </c>
+      <c r="G92">
+        <v>4169.8999999999996</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
       <c r="A93">
         <v>91</v>
       </c>
@@ -4891,8 +5723,17 @@
       <c r="C93">
         <v>4586.3999999999996</v>
       </c>
-    </row>
-    <row r="94" spans="1:3">
+      <c r="E93">
+        <v>91</v>
+      </c>
+      <c r="F93">
+        <v>45959</v>
+      </c>
+      <c r="G93">
+        <v>4253.2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
       <c r="A94">
         <v>92</v>
       </c>
@@ -4902,8 +5743,17 @@
       <c r="C94">
         <v>4620.7</v>
       </c>
-    </row>
-    <row r="95" spans="1:3">
+      <c r="E94">
+        <v>92</v>
+      </c>
+      <c r="F94">
+        <v>46464</v>
+      </c>
+      <c r="G94">
+        <v>4331.6000000000004</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
       <c r="A95">
         <v>93</v>
       </c>
@@ -4913,8 +5763,17 @@
       <c r="C95">
         <v>4689.3</v>
       </c>
-    </row>
-    <row r="96" spans="1:3">
+      <c r="E95">
+        <v>93</v>
+      </c>
+      <c r="F95">
+        <v>46969</v>
+      </c>
+      <c r="G95">
+        <v>4419.8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
       <c r="A96">
         <v>94</v>
       </c>
@@ -4924,8 +5783,17 @@
       <c r="C96">
         <v>4738.3</v>
       </c>
-    </row>
-    <row r="97" spans="1:3">
+      <c r="E96">
+        <v>94</v>
+      </c>
+      <c r="F96">
+        <v>47474</v>
+      </c>
+      <c r="G96">
+        <v>4503.1000000000004</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
       <c r="A97">
         <v>95</v>
       </c>
@@ -4935,8 +5803,17 @@
       <c r="C97">
         <v>4787.3</v>
       </c>
-    </row>
-    <row r="98" spans="1:3">
+      <c r="E97">
+        <v>95</v>
+      </c>
+      <c r="F97">
+        <v>47979</v>
+      </c>
+      <c r="G97">
+        <v>4591.3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
       <c r="A98">
         <v>96</v>
       </c>
@@ -4946,8 +5823,17 @@
       <c r="C98">
         <v>4846.1000000000004</v>
       </c>
-    </row>
-    <row r="99" spans="1:3">
+      <c r="E98">
+        <v>96</v>
+      </c>
+      <c r="F98">
+        <v>48484</v>
+      </c>
+      <c r="G98">
+        <v>4684.3999999999996</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
       <c r="A99">
         <v>97</v>
       </c>
@@ -4957,8 +5843,17 @@
       <c r="C99">
         <v>4895.1000000000004</v>
       </c>
-    </row>
-    <row r="100" spans="1:3">
+      <c r="E99">
+        <v>97</v>
+      </c>
+      <c r="F99">
+        <v>48989</v>
+      </c>
+      <c r="G99">
+        <v>4777.5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
       <c r="A100">
         <v>98</v>
       </c>
@@ -4968,8 +5863,17 @@
       <c r="C100">
         <v>4944.1000000000004</v>
       </c>
-    </row>
-    <row r="101" spans="1:3">
+      <c r="E100">
+        <v>98</v>
+      </c>
+      <c r="F100">
+        <v>49494</v>
+      </c>
+      <c r="G100">
+        <v>4875.5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
       <c r="A101">
         <v>99</v>
       </c>
@@ -4978,6 +5882,15 @@
       </c>
       <c r="C101">
         <v>4998</v>
+      </c>
+      <c r="E101">
+        <v>99</v>
+      </c>
+      <c r="F101">
+        <v>50000</v>
+      </c>
+      <c r="G101">
+        <v>4968.6000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>